<commit_message>
improve the DDL script and complete CRUD
</commit_message>
<xml_diff>
--- a/CRUDtable.xlsx
+++ b/CRUDtable.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John-Dao\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John-Dao\workspace\DAT602-Milestone-1-Quang-Thanh-Dao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76E9D551-3CCD-456D-BF31-93B80DDDA9C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5D1D2E5-32B6-43D5-A3EE-5D87921D7B3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11385" xr2:uid="{C9D736BE-ED9B-47FD-9C53-5EE62E929E58}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C9D736BE-ED9B-47FD-9C53-5EE62E929E58}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="79">
   <si>
     <t>CRUD for tile based game.</t>
   </si>
@@ -68,9 +68,6 @@
     <t>U</t>
   </si>
   <si>
-    <t>Remove Player</t>
-  </si>
-  <si>
     <t>Table</t>
   </si>
   <si>
@@ -83,9 +80,6 @@
     <t>R,D</t>
   </si>
   <si>
-    <t>Score</t>
-  </si>
-  <si>
     <t>Collect Item</t>
   </si>
   <si>
@@ -251,9 +245,6 @@
     <t>Edit User</t>
   </si>
   <si>
-    <t>Remove User</t>
-  </si>
-  <si>
     <t>Table User, Character, Session</t>
   </si>
   <si>
@@ -273,6 +264,12 @@
   </si>
   <si>
     <t>Table Chat</t>
+  </si>
+  <si>
+    <t>Remove/Delete Player</t>
+  </si>
+  <si>
+    <t>Gain new high score</t>
   </si>
 </sst>
 </file>
@@ -428,7 +425,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -458,19 +455,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -482,8 +473,20 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -802,25 +805,25 @@
   <dimension ref="A1:AJ34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.28515625" customWidth="1"/>
-    <col min="24" max="24" width="10.28515625" customWidth="1"/>
-    <col min="26" max="26" width="10.140625" customWidth="1"/>
-    <col min="31" max="31" width="11.5703125" customWidth="1"/>
-    <col min="33" max="33" width="10.28515625" customWidth="1"/>
-    <col min="35" max="35" width="10.140625" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="24" max="24" width="10.33203125" customWidth="1"/>
+    <col min="26" max="26" width="10.109375" customWidth="1"/>
+    <col min="31" max="31" width="11.5546875" customWidth="1"/>
+    <col min="33" max="33" width="10.33203125" customWidth="1"/>
+    <col min="35" max="35" width="10.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
         <v>2</v>
       </c>
@@ -834,19 +837,19 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
       <c r="C3" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="W3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -858,7 +861,7 @@
       <c r="K4" s="11"/>
       <c r="L4" s="9"/>
       <c r="M4" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
@@ -866,136 +869,136 @@
       <c r="Q4" s="4"/>
       <c r="R4" s="9"/>
       <c r="S4" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="T4" s="4"/>
       <c r="U4" s="4"/>
       <c r="V4" s="4"/>
       <c r="W4" s="9"/>
       <c r="X4" s="13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="Y4" s="14"/>
       <c r="Z4" s="14"/>
       <c r="AA4" s="14"/>
       <c r="AB4" s="9"/>
       <c r="AC4" s="13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="AD4" s="14"/>
       <c r="AE4" s="14"/>
       <c r="AF4" s="9"/>
       <c r="AG4" s="13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="AH4" s="14"/>
       <c r="AI4" s="14"/>
       <c r="AJ4" s="14"/>
     </row>
-    <row r="5" spans="1:36" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="G5" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="H5" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" s="5" t="s">
+      <c r="I5" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>36</v>
-      </c>
       <c r="J5" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="L5" s="10"/>
       <c r="M5" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="O5" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="P5" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="P5" s="6" t="s">
-        <v>40</v>
-      </c>
       <c r="Q5" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="R5" s="10"/>
       <c r="S5" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="T5" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="U5" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="T5" s="6" t="s">
+      <c r="V5" s="6" t="s">
         <v>43</v>
-      </c>
-      <c r="U5" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="V5" s="6" t="s">
-        <v>45</v>
       </c>
       <c r="W5" s="10"/>
       <c r="X5" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y5" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="Y5" s="7" t="s">
-        <v>50</v>
-      </c>
       <c r="Z5" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA5" s="7" t="s">
         <v>49</v>
-      </c>
-      <c r="AA5" s="7" t="s">
-        <v>51</v>
       </c>
       <c r="AB5" s="10"/>
       <c r="AC5" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD5" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE5" s="7" t="s">
         <v>52</v>
-      </c>
-      <c r="AD5" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="AE5" s="7" t="s">
-        <v>54</v>
       </c>
       <c r="AF5" s="10"/>
       <c r="AG5" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH5" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI5" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="AH5" s="7" t="s">
+      <c r="AJ5" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="AI5" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="AJ5" s="7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>1</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>6</v>
@@ -1050,7 +1053,7 @@
       <c r="AI6" s="1"/>
       <c r="AJ6" s="1"/>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <f>A6+1</f>
         <v>2</v>
@@ -1060,17 +1063,17 @@
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>8</v>
@@ -1103,7 +1106,7 @@
       <c r="AI7" s="1"/>
       <c r="AJ7" s="1"/>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <f t="shared" ref="A8:A19" si="0">A7+1</f>
         <v>3</v>
@@ -1115,18 +1118,18 @@
         <v>8</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>8</v>
@@ -1158,69 +1161,69 @@
       <c r="AI8" s="1"/>
       <c r="AJ8" s="1"/>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:36" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>11</v>
+      <c r="B9" s="22" t="s">
+        <v>77</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="L9" s="10"/>
       <c r="M9" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="R9" s="10"/>
       <c r="S9" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="T9" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="U9" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="V9" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="W9" s="12"/>
       <c r="X9" s="1"/>
@@ -1237,13 +1240,13 @@
       <c r="AI9" s="1"/>
       <c r="AJ9" s="1"/>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -1290,13 +1293,13 @@
       <c r="AI10" s="1"/>
       <c r="AJ10" s="1"/>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -1317,16 +1320,16 @@
       <c r="Q11" s="1"/>
       <c r="R11" s="9"/>
       <c r="S11" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="T11" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="U11" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="V11" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="W11" s="9"/>
       <c r="X11" s="1"/>
@@ -1343,13 +1346,13 @@
       <c r="AI11" s="1"/>
       <c r="AJ11" s="1"/>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -1364,23 +1367,23 @@
         <v>10</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="L12" s="9"/>
       <c r="M12" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="R12" s="9"/>
       <c r="S12" s="1"/>
@@ -1404,13 +1407,13 @@
       <c r="AI12" s="1"/>
       <c r="AJ12" s="1"/>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -1420,7 +1423,7 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K13" s="1"/>
       <c r="L13" s="9"/>
@@ -1471,13 +1474,13 @@
       <c r="AI13" s="1"/>
       <c r="AJ13" s="1"/>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -1492,32 +1495,32 @@
       <c r="K14" s="1"/>
       <c r="L14" s="9"/>
       <c r="M14" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="R14" s="9"/>
       <c r="S14" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="T14" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="U14" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="V14" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="W14" s="9"/>
       <c r="X14" s="1"/>
@@ -1534,13 +1537,13 @@
       <c r="AI14" s="1"/>
       <c r="AJ14" s="1"/>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:36" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>16</v>
+      <c r="B15" s="22" t="s">
+        <v>78</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -1551,7 +1554,7 @@
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="L15" s="9"/>
       <c r="M15" s="1"/>
@@ -1583,13 +1586,13 @@
       <c r="AI15" s="1"/>
       <c r="AJ15" s="1"/>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -1606,7 +1609,7 @@
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
       <c r="Q16" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="R16" s="9"/>
       <c r="S16" s="1"/>
@@ -1618,7 +1621,7 @@
       <c r="Y16" s="1"/>
       <c r="Z16" s="1"/>
       <c r="AA16" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AB16" s="9"/>
       <c r="AC16" s="1"/>
@@ -1630,13 +1633,13 @@
       <c r="AI16" s="1"/>
       <c r="AJ16" s="1"/>
     </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <f>A16+1</f>
         <v>12</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -1651,7 +1654,7 @@
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
       <c r="O17" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
@@ -1683,13 +1686,13 @@
       <c r="AI17" s="1"/>
       <c r="AJ17" s="1"/>
     </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -1703,7 +1706,7 @@
       <c r="L18" s="9"/>
       <c r="M18" s="1"/>
       <c r="N18" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
@@ -1718,7 +1721,7 @@
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
       <c r="AA18" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AB18" s="9"/>
       <c r="AC18" s="1"/>
@@ -1730,13 +1733,13 @@
       <c r="AI18" s="1"/>
       <c r="AJ18" s="1"/>
     </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -1781,197 +1784,191 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1</v>
       </c>
       <c r="B21" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="C21" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="C21" s="27" t="s">
-        <v>68</v>
-      </c>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
       <c r="J21" s="8"/>
     </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="C22" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="D22" s="26"/>
-      <c r="E22" s="26"/>
-    </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="C22" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
+    </row>
+    <row r="23" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>3</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="C23" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
-    </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="C23" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="D23" s="30"/>
+      <c r="E23" s="30"/>
+    </row>
+    <row r="24" spans="1:36" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>4</v>
       </c>
-      <c r="B24" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="C24" s="29" t="s">
-        <v>73</v>
-      </c>
-      <c r="D24" s="29"/>
-      <c r="E24" s="29"/>
-    </row>
-    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="B24" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="C24" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="D24" s="27"/>
+      <c r="E24" s="27"/>
+    </row>
+    <row r="25" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>5</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="C25" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="D25" s="30"/>
-      <c r="E25" s="30"/>
-    </row>
-    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="C25" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="D25" s="28"/>
+      <c r="E25" s="28"/>
+    </row>
+    <row r="26" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>6</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="C26" s="23" t="s">
-        <v>75</v>
-      </c>
-      <c r="D26" s="23"/>
-      <c r="E26" s="23"/>
-    </row>
-    <row r="27" spans="1:36" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="C26" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="D26" s="25"/>
+      <c r="E26" s="25"/>
+    </row>
+    <row r="27" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>7</v>
       </c>
       <c r="B27" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="C27" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-    </row>
-    <row r="28" spans="1:36" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="C27" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
+    </row>
+    <row r="28" spans="1:36" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>8</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C28" s="31" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D28" s="31"/>
       <c r="E28" s="31"/>
     </row>
-    <row r="29" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>9</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="C29" s="29" t="s">
-        <v>73</v>
-      </c>
-      <c r="D29" s="29"/>
-      <c r="E29" s="29"/>
-    </row>
-    <row r="30" spans="1:36" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="C29" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+    </row>
+    <row r="30" spans="1:36" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>10</v>
       </c>
-      <c r="B30" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="C30" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="D30" s="30"/>
-      <c r="E30" s="30"/>
-    </row>
-    <row r="31" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="B30" s="33" t="s">
+        <v>78</v>
+      </c>
+      <c r="C30" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="D30" s="28"/>
+      <c r="E30" s="28"/>
+    </row>
+    <row r="31" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>11</v>
       </c>
       <c r="B31" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="C31" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="D31" s="23"/>
-      <c r="E31" s="23"/>
-    </row>
-    <row r="32" spans="1:36" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="C31" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="D31" s="25"/>
+      <c r="E31" s="25"/>
+    </row>
+    <row r="32" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>12</v>
       </c>
       <c r="B32" t="s">
-        <v>19</v>
-      </c>
-      <c r="C32" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="D32" s="24"/>
-      <c r="E32" s="24"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="C32" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="D32" s="29"/>
+      <c r="E32" s="29"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>13</v>
       </c>
       <c r="B33" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="C33" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="D33" s="23"/>
-      <c r="E33" s="23"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="C33" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="D33" s="25"/>
+      <c r="E33" s="25"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>14</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="C34" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="D34" s="25"/>
-      <c r="E34" s="25"/>
+        <v>20</v>
+      </c>
+      <c r="C34" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="D34" s="30"/>
+      <c r="E34" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="C25:E25"/>
     <mergeCell ref="C31:E31"/>
     <mergeCell ref="C32:E32"/>
     <mergeCell ref="C33:E33"/>
@@ -1980,6 +1977,12 @@
     <mergeCell ref="C29:E29"/>
     <mergeCell ref="C30:E30"/>
     <mergeCell ref="C28:E28"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C25:E25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>
@@ -1996,6 +1999,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C13B0570F2253F43A8935F018FB9D300" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="34193cf9432cb2f5c040bcc38715d5e4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a487797b-6e19-4ce8-9c67-927f03bd870c" xmlns:ns4="6a7c71a7-f1a2-410a-a683-e07a7dae386f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8e9bff7d7b429ca3622085fa43548888" ns3:_="" ns4:_="">
     <xsd:import namespace="a487797b-6e19-4ce8-9c67-927f03bd870c"/>
@@ -2212,12 +2221,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1A8BDFE-6EDD-47FA-8333-F416F3CEF24B}">
   <ds:schemaRefs>
@@ -2227,6 +2230,15 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B47D9897-91FC-4918-B3B0-E96EAE152C25}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D3AF6CE-D761-46A2-B970-2593752294FB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2243,13 +2255,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B47D9897-91FC-4918-B3B0-E96EAE152C25}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>